<commit_message>
added more visualisations and improved the filtering
</commit_message>
<xml_diff>
--- a/data/test_collection_with_abstracts.xlsx
+++ b/data/test_collection_with_abstracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei.aioanei/Documents/GitHub/semantic-papers-filter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F488F5E-D80B-0E4B-B08B-05D3245B515A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E5CB90-F7CF-7140-8EC7-B7502158753D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="174">
   <si>
     <t>PMID</t>
   </si>
@@ -3373,42 +3373,6 @@
     <t>Ground Method Name</t>
   </si>
   <si>
-    <t>Is Relevant</t>
-  </si>
-  <si>
-    <t>Method Type</t>
-  </si>
-  <si>
-    <t>Method Name</t>
-  </si>
-  <si>
-    <t>{'architecture': 0.0, 'task': 0.0}</t>
-  </si>
-  <si>
-    <t>{'architecture': 1.0, 'context': 1.0, 'task': 1.0}</t>
-  </si>
-  <si>
-    <t>{'context': 1.0, 'architecture': 1.0, 'task': 0.5}</t>
-  </si>
-  <si>
-    <t>{'architecture': 0.0, 'task': 0.0, 'context': 0.0}</t>
-  </si>
-  <si>
-    <t>{'task': 1.0, 'context': 0.75, 'architecture': 0.0}</t>
-  </si>
-  <si>
-    <t>{'context': 0.5, 'architecture': 0.0, 'task': 0.0}</t>
-  </si>
-  <si>
-    <t>{'architecture': 1.0, 'context': 0.5, 'task': 0.5}</t>
-  </si>
-  <si>
-    <t>{'context': 0.5, 'task': 1.0, 'architecture': 0.0}</t>
-  </si>
-  <si>
-    <t>{'task': 0.5, 'architecture': 0.0, 'context': 0.0}</t>
-  </si>
-  <si>
     <t>Inceptionv3 neural networks</t>
   </si>
   <si>
@@ -5719,215 +5683,519 @@
     </r>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>pathology approach, media technique, testing dataset, technique, computer approach, vision approach, kidney approach, thickness study, training framework, approach, sampling, pathology characterize, framework, intima technique, intima made, deep learning</t>
-  </si>
-  <si>
-    <t>encoder module, input architecture, decoder architecture, MD architecture, encoder, decoder, module, aggregation architecture, feature module, lesion module, architecture, lesion architecture, decoder module, treatment strategies, strategies, deep-learning</t>
-  </si>
-  <si>
-    <t>cohort, protocol, ST models, ST for, performance quantify, sections, III cohort, neural network, cancer cohort, deep learning, grade sections, Inceptionv3, protocols, slide images, ST studies, models, T cohort, Stage cohort, images</t>
-  </si>
-  <si>
-    <t>plasmid strategy, cnn, capture as, microscopy, field microscopy, phages, M13 strategy, M13 phages, convolutional neural network, network, systems, field network, neural network, strategy</t>
-  </si>
-  <si>
-    <t>χ2 test, machine learning, rank test, NLST codes, ai model, sum test, CT identify, artificial intelligence, Pearson test</t>
-  </si>
-  <si>
-    <t>requirements, e in, health detect, Synthetic Warnings, - in, Health Warnings, cigarette brands, e brands, Synthetic nicotine, media, - brands, cigarette in, regression analyses, Instagram Warnings, health requirements, health evaluate, Nicotine Warnings, user evaluate, warning requirements, tobacco manufacturers</t>
-  </si>
-  <si>
-    <t>CAM tool, learning approach, CoV-2 approach, approach, Grad tool, CNN, cnn, HIV-1 model, SARS applied, CoV-2 applied, interpretability tool, phase approach, gan, SARS spectrograms, VGG-16 model, HIV-1 applied, tool, vgg, SARS to, transfer approach, CoV-2 spectrograms, transfer learning, spectrograms, model, SARS approach, VGG-16 applied, CoV-2 to</t>
-  </si>
-  <si>
-    <t>lung framework, step framework, system, size strategies, feature framework, point framework, framework, size for, chest, chest framework, radiographs, artificial intelligence, transplant framework, lung for, recipient reduce, mask framework, deep learning</t>
-  </si>
-  <si>
-    <t>learning method, Seg-CycleGAN, network, transfer method, kidney generate, strategy, segmentation method, segmentation obtain, kidney method, Seg network, tomography generate, gan, Transfer Learning Based, method, US method, translation network, image in, kidney in, transfer learning, US generate, deep-learning</t>
-  </si>
-  <si>
-    <t>learning compare, network model, Google model, Google images, window model, design features, convolutional neural network, Street model, neural model, Street images, View model, case model, computer model, neural network, deep learning, machine features, machine learning, features, Deep Learning Approach Passive, model, vision model, case as, learning features, images, View images, machine compare</t>
-  </si>
-  <si>
-    <t>information, foundation model, gpt, artificial intelligence</t>
-  </si>
-  <si>
-    <t>composition facilitate, SliceOmatic, plots, source AutoMATiCA, Bland plots, AutoMATiCA, correlation plots, body facilitate, tomography</t>
-  </si>
-  <si>
-    <t>statistics, basement from, N=254/266 in, PAS in, disease select, NEPTUNE in, Redundancy Relevance, proteinuria select, change from, CureGN from, image segmentations, deep-learning, Maximum Relevance, summary statistics</t>
-  </si>
-  <si>
-    <t>method, encoder, thickness to, autoencoder, scanners, methods, models, variational autoencoder, deep learning</t>
-  </si>
-  <si>
-    <t>OS framework, approach, regression method, regression network, segmentation framework, tumor framework, input approach, resonance method, survival without, window approach, tumor focusing, learning framework, tumor with, feature map, brain framework, method, map, unet, brain method, framework, matrix approach, survival network, resonance imaging, imaging leverage, brain with, imaging</t>
-  </si>
-  <si>
-    <t>learning implementing, study study, machine learning, them, methods, study principles, artificial intelligence, learning methods, neural network, deep learning</t>
-  </si>
-  <si>
-    <t>cnn, Feature network, EPC predict, deep neural, Regulatory network, Convolutional Neural Network, Matrix network, Gene network, Gene Regulatory Network, convolutional neural network, EPC infer, SVCV infer, network, SVCV predict, CNN, Network network, gan, neural network</t>
-  </si>
-  <si>
-    <t>control design, study study, design, case control, study design, control control, TCGA dataset, case design</t>
-  </si>
-  <si>
-    <t>uncertainty estimation, Deep, Instance method, instance in, test on, method, estimation, MIL reducing, neural suffered, artificial intelligence, training acquire, neural network, deep learning</t>
-  </si>
-  <si>
-    <t>Scores</t>
-  </si>
-  <si>
-    <t>{'context': 0.25, 'architecture': 1.0}</t>
-  </si>
-  <si>
-    <t>{'task': 1.0, 'architecture': 1.0, 'context': 0.75}</t>
-  </si>
-  <si>
-    <t>{'task': 1.0, 'architecture': 1.0, 'context': 0.25}</t>
-  </si>
-  <si>
-    <t>{'architecture': 1.0, 'context': 1.0, 'task': 0.5}</t>
-  </si>
-  <si>
-    <t>{'architecture': 1.0, 'context': 0.25, 'task': 1.0}</t>
-  </si>
-  <si>
-    <t>{'context': 0.25, 'task': 0.5, 'architecture': 0.0}</t>
-  </si>
-  <si>
-    <t>{'context': 0.25, 'architecture': 0.0, 'task': 0.0}</t>
-  </si>
-  <si>
-    <t>{'context': 0.25, 'architecture': 1.0, 'task': 0.5}</t>
-  </si>
-  <si>
-    <t>{'context': 1.0, 'architecture': 1.0}</t>
-  </si>
-  <si>
-    <t>{'task': 1.0, 'context': 1.0, 'architecture': 1.0}</t>
-  </si>
-  <si>
-    <t>Similarity Scores</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.3659791946411133}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.3273022472858429}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.38244327902793884}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.2876262366771698}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.1125103160738945}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.271595299243927}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.1729719340801239}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.28861474990844727}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.16059540212154388}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.19433438777923584}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.15445350110530853}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.2840840220451355}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.3966098725795746}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.3372344672679901}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.3862060010433197}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.4156630337238312}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.08572600781917572}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.33280929923057556}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.2853389084339142}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.1921899914741516}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.14596182107925415}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.11709101498126984}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.18362507224082947}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.25520724058151245}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.16349175572395325}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.39128535985946655}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.11896203458309174}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.29435834288597107}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.274456262588501}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.15291376411914825}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.48958808183670044}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.30693885684013367}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.16575561463832855}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.17195454239845276}</t>
-  </si>
-  <si>
-    <t>{'similarity': 0.37379103899002075}</t>
-  </si>
-  <si>
-    <t>Is Relevant by Similarity</t>
+    <t>38956213</t>
+  </si>
+  <si>
+    <t>The severity of dry eye symptoms and risk factors among university students in Saudi Arabia: a cross-sectional study</t>
+  </si>
+  <si>
+    <t>Dry eye syndrome (DES) is a tear film disorder caused by increased tear evaporation or decreased production. The heavy workload on the eye and the increased usage of digital screens may decrease blink frequency, leading to an increased evaporation rate and an upsurge in the incidence and severity of DES. This study aims to assess the severity of DES symptoms and the risk factors among university students. A cross-sectional study was conducted at Umm AlQura University to evaluate the severity of DES among students and explore its potential association with digital screen use. Validated questionnaires were used to assess the severity of DES and digital screen usage. The study included 457 participants, of which 13% had symptoms suggestive of severe DES. Furthermore, multiple risk factors had a significant association with the severity of DES, including gender, use of monitor filters, monitor and room brightness, and smoking habits. DES symptoms were prevalent among university students, particularly female students. Although there was no significant association with the duration of screen usage and collage distribution. Other factors however, such as the usage of screen monitors and the brightness of both the monitor and the room, were significantly associated with the severity of DES symptoms.</t>
+  </si>
+  <si>
+    <t>38935799</t>
+  </si>
+  <si>
+    <t>ST-CellSeg: Cell segmentation for imaging-based spatial transcriptomics using multi-scale manifold learning</t>
+  </si>
+  <si>
+    <t>PLoS Comput Biol</t>
+  </si>
+  <si>
+    <t>38934830</t>
+  </si>
+  <si>
+    <t>Prevalence and Association of Digital Eye Strain with the Quality of Sleep and Feeling of Loneliness among Female College Students in Northern India</t>
+  </si>
+  <si>
+    <t>Indian J Public Health</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>INTRODUCTION: Because of COVID's impact on social behavior, students have become more reliant on computer-facilitated communication to continue their studies and interact with friends. While it is known that the association between screen exposure and psychological well-being is both harmful and stronger among adolescents than younger children, what is less studied are the causal factors that may mediate the relationship.
+OBJECTIVES: The objectives of this study were to analyze the relationship between screen exposure and two psychological outcomes, sleep quality and loneliness, using digital eye strain as a mediating factor. Eye strain is expected to have a direct and harmful influence on psychological well-being.
+MATERIALS AND METHODS: A structured and validated questionnaire was transcribed and administered online. A nonrepresentative sample of 497 female college students in a North Indian city participated in the study. Digital eye strain, quality of sleep, and feeling of loneliness scores were assessed using latent class analysis.
+RESULTS: The selected latent model suggested that Class 2 had a high percentage of students with network issues, the problem with space and noise, and various financial hardships, which had almost doubled the rate of loneliness (53.28%) and sleep-wake difficulties (75.41%) among the students affected with computer vision syndrome (89.75%).
+CONCLUSION: There is an urgent need to examine the implications of digital exposure across gender and age to prevent future complications. Further, awareness for improving holistic well-being in the digital era should be promoted through various platforms.</t>
+  </si>
+  <si>
+    <t>38926396</t>
+  </si>
+  <si>
+    <t>ROCOv2: Radiology Objects in COntext Version 2, an Updated Multimodal Image Dataset</t>
+  </si>
+  <si>
+    <t>Sci Data</t>
+  </si>
+  <si>
+    <t>38925254</t>
+  </si>
+  <si>
+    <t>AI-based opportunistic quantitative image analysis of lung cancer screening CTs to reduce disparities in osteoporosis screening</t>
+  </si>
+  <si>
+    <t>Bone</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spatial transcriptomics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> has gained popularity over the past decade due to its ability to evaluate transcriptome data while preserving spatial information. Cell </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segmentation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a crucial step in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spatial transcriptomic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> analysis, as it enables the avoidance of unpredictable tissue disentanglement steps. Although high-quality </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cell segmentation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> algorithms can aid in the extraction of valuable data, traditional methods are frequently non-spatial, do not account for spatial information efficiently, and perform poorly when confronted with the problem of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spatial transcriptome cell segmentation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with varying shapes. In this study, we propose ST-CellSeg, an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>image-based machine learning method for spatial transcriptomics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that uses manifold for cell </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segmentation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and is novel in its consideration of multi-scale information. We first construct a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fully connected graph</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which acts as a spatial transcriptomic manifold. Using multi-scale data, we then determine the low-dimensional </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spatial probability distribution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> representation for cell </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segmentation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Using the adjusted Rand index (ARI), normalized mutual information (NMI), and Silhouette coefficient (SC) as model performance measures, the proposed algorithm significantly outperforms baseline models in selected datasets and is efficient in computational complexity.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Automated medical </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>image analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> systems often require large amounts of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>training data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with high quality labels, which are difficult and time consuming to generate. This paper introduces Radiology Object in COntext version 2 (ROCOv2), a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>multimodal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dataset consisting of radiological images and associated medical concepts and captions extracted from the PMC Open Access subset. It is an updated version of the ROCO dataset published in 2018, and adds 35,705 new images added to PMC since 2018. It further provides manually curated concepts for imaging modalities with additional anatomical and directional concepts for X-rays. The dataset consists of 79,789 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>images</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and has been used, with minor modifications, in the concept </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>detection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and caption prediction tasks of ImageCLEFmedical Caption 2023. The dataset is suitable for training</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> image annotation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> models based on image-caption pairs, or for multi-label </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>image classification</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> using Unified Medical Language System (UMLS) concepts provided with each image. In addition, it can serve for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pre-training</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of medical domain models, and evaluation of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deep learning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> models for multi-task learning.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Osteoporosis is underdiagnosed, especially in ethnic and racial minorities who are thought to be protected against bone loss, but often have worse outcomes after an osteoporotic fracture. We aimed to determine the prevalence of osteoporosis by opportunistic CT in patients who underwent lung cancer screening (LCS) using non-contrast CT in the Northeastern United States. Demographics including race and ethnicity were retrieved. We assessed trabecular bone and body composition using a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fully-automated artificial intelligence algorithm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. ROIs were placed at T12 vertebral body for attenuation measurements in Hounsfield Units (HU). Two validated thresholds were used to diagnose osteoporosis: high-sensitivity threshold (115-165 HU) and high specificity threshold (&lt;115 HU). We performed descriptive statistics and ANOVA to compare differences across sex, race, ethnicity, and income class according to neighborhoods' mean household incomes. Forward stepwise </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">regression modeling </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>was used to determine body composition predictors of trabecular attenuation. We included 3708 patients (mean age 64 ± 7 years, 54 % males) who underwent LCS, had available demographic information and an evaluable CT for trabecular attenuation analysis. Using the high sensitivity threshold, osteoporosis was more prevalent in females (74 % vs. 65 % in males, p &lt; 0.0001) and Whites (72 % vs 49 % non-Whites, p &lt; 0.0001). However, osteoporosis was present across all races (38 % Black, 55 % Asian, 56 % Hispanic) and affected all income classes (69 %, 69 %, and 91 % in low, medium, and high-income class, respectively). High visceral/subcutaneous fat-ratio, aortic calcification, and hepatic steatosis were associated with low trabecular attenuation (p &lt; 0.01), whereas muscle mass was positively associated with trabecular attenuation (p &lt; 0.01). In conclusion, osteoporosis is prevalent across all races, income classes and both sexes in patients undergoing LCS. Opportunistic CT using a fully-automated algorithm and uniform imaging protocol is able to detect osteoporosis and body composition without additional testing or radiation. Early identification of patients traditionally thought to be at low risk for bone loss will allow for initiating appropriate treatment to prevent future fragility fractures. CLINICALTRIALS.GOV IDENTIFIER: N/A.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5949,12 +6217,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -6044,16 +6306,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6358,31 +6620,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="49.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="107.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="8" customWidth="1"/>
     <col min="8" max="8" width="27.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" customWidth="1"/>
-    <col min="11" max="11" width="124.1640625" customWidth="1"/>
-    <col min="12" max="12" width="59.5" customWidth="1"/>
-    <col min="13" max="13" width="40.5" customWidth="1"/>
-    <col min="14" max="14" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6401,32 +6657,14 @@
       <c r="F1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>105</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>233</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -6442,20 +6680,8 @@
       <c r="F2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>110</v>
-      </c>
-      <c r="M2" t="s">
-        <v>198</v>
-      </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" ht="259" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="259" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -6474,32 +6700,14 @@
       <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" t="s">
-        <v>167</v>
-      </c>
-      <c r="L3" t="s">
-        <v>187</v>
-      </c>
-      <c r="M3" t="s">
-        <v>199</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" ht="233" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="233" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -6518,32 +6726,14 @@
       <c r="F4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>81</v>
-      </c>
-      <c r="K4" t="s">
-        <v>168</v>
-      </c>
-      <c r="L4" t="s">
-        <v>116</v>
-      </c>
-      <c r="M4" t="s">
-        <v>200</v>
-      </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:14" ht="332" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="332" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -6562,32 +6752,14 @@
       <c r="F5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K5" t="s">
-        <v>169</v>
-      </c>
-      <c r="L5" t="s">
-        <v>112</v>
-      </c>
-      <c r="M5" t="s">
-        <v>201</v>
-      </c>
-      <c r="N5" t="b">
-        <v>0</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -6606,32 +6778,14 @@
       <c r="F6" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" t="s">
-        <v>170</v>
-      </c>
-      <c r="L6" t="s">
-        <v>188</v>
-      </c>
-      <c r="M6" t="s">
-        <v>202</v>
-      </c>
-      <c r="N6" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:14" ht="304" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="304" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -6650,32 +6804,14 @@
       <c r="F7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K7" t="s">
-        <v>171</v>
-      </c>
-      <c r="L7" t="s">
-        <v>188</v>
-      </c>
-      <c r="M7" t="s">
-        <v>203</v>
-      </c>
-      <c r="N7" t="b">
-        <v>0</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="192" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -6694,20 +6830,8 @@
       <c r="F8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>113</v>
-      </c>
-      <c r="M8" t="s">
-        <v>204</v>
-      </c>
-      <c r="N8" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:14" ht="176" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -6721,25 +6845,13 @@
         <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>110</v>
-      </c>
-      <c r="M9" t="s">
-        <v>205</v>
-      </c>
-      <c r="N9" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:14" ht="192" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -6758,20 +6870,8 @@
       <c r="F10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>110</v>
-      </c>
-      <c r="M10" t="s">
-        <v>206</v>
-      </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:14" ht="365" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="365" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -6790,29 +6890,11 @@
       <c r="F11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>87</v>
-      </c>
-      <c r="K11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L11" t="s">
-        <v>117</v>
-      </c>
-      <c r="M11" t="s">
-        <v>207</v>
-      </c>
-      <c r="N11" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:14" ht="259" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="259" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -6831,20 +6913,8 @@
       <c r="F12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>115</v>
-      </c>
-      <c r="M12" t="s">
-        <v>208</v>
-      </c>
-      <c r="N12" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:14" ht="212" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="212" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -6863,29 +6933,11 @@
       <c r="F13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" t="s">
-        <v>173</v>
-      </c>
-      <c r="L13" t="s">
-        <v>189</v>
-      </c>
-      <c r="M13" t="s">
-        <v>209</v>
-      </c>
-      <c r="N13" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:14" ht="164" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="164" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -6904,20 +6956,8 @@
       <c r="F14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" t="s">
-        <v>110</v>
-      </c>
-      <c r="M14" t="s">
-        <v>210</v>
-      </c>
-      <c r="N14" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:14" ht="180" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="180" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -6936,29 +6976,11 @@
       <c r="F15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" t="s">
-        <v>174</v>
-      </c>
-      <c r="L15" t="s">
-        <v>116</v>
-      </c>
-      <c r="M15" t="s">
-        <v>211</v>
-      </c>
-      <c r="N15" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:14" ht="261" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="261" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -6977,29 +6999,11 @@
       <c r="F16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K16" t="s">
-        <v>175</v>
-      </c>
-      <c r="L16" t="s">
-        <v>190</v>
-      </c>
-      <c r="M16" t="s">
-        <v>212</v>
-      </c>
-      <c r="N16" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:14" ht="182" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="182" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -7018,29 +7022,11 @@
       <c r="F17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>81</v>
-      </c>
-      <c r="K17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L17" t="s">
-        <v>111</v>
-      </c>
-      <c r="M17" t="s">
-        <v>213</v>
-      </c>
-      <c r="N17" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="18" spans="1:14" ht="224" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -7059,20 +7045,8 @@
       <c r="F18" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" t="s">
-        <v>110</v>
-      </c>
-      <c r="M18" t="s">
-        <v>214</v>
-      </c>
-      <c r="N18" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="19" spans="1:14" ht="185" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="185" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -7086,37 +7060,19 @@
         <v>8</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F19" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="8" t="s">
         <v>87</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>87</v>
-      </c>
-      <c r="K19" t="s">
-        <v>177</v>
-      </c>
-      <c r="L19" t="s">
-        <v>191</v>
-      </c>
-      <c r="M19" t="s">
-        <v>215</v>
-      </c>
-      <c r="N19" t="b">
-        <v>0</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="151" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -7130,25 +7086,13 @@
         <v>8</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="F20" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>110</v>
-      </c>
-      <c r="M20" t="s">
-        <v>216</v>
-      </c>
-      <c r="N20" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="21" spans="1:14" ht="244" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="244" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
@@ -7162,34 +7106,16 @@
         <v>8</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="s">
-        <v>81</v>
-      </c>
-      <c r="K21" t="s">
-        <v>178</v>
-      </c>
-      <c r="L21" t="s">
-        <v>192</v>
-      </c>
-      <c r="M21" t="s">
-        <v>217</v>
-      </c>
-      <c r="N21" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="22" spans="1:14" ht="288" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
@@ -7208,20 +7134,8 @@
       <c r="F22" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>118</v>
-      </c>
-      <c r="M22" t="s">
-        <v>218</v>
-      </c>
-      <c r="N22" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="23" spans="1:14" ht="304" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="304" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -7240,20 +7154,8 @@
       <c r="F23" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>110</v>
-      </c>
-      <c r="M23" t="s">
-        <v>219</v>
-      </c>
-      <c r="N23" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="24" spans="1:14" ht="256" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>71</v>
       </c>
@@ -7272,20 +7174,8 @@
       <c r="F24" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>110</v>
-      </c>
-      <c r="M24" t="s">
-        <v>220</v>
-      </c>
-      <c r="N24" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="25" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
@@ -7304,29 +7194,11 @@
       <c r="F25" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" t="s">
-        <v>81</v>
-      </c>
-      <c r="K25" t="s">
-        <v>179</v>
-      </c>
-      <c r="L25" t="s">
-        <v>187</v>
-      </c>
-      <c r="M25" t="s">
-        <v>221</v>
-      </c>
-      <c r="N25" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="26" spans="1:14" ht="288" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
@@ -7345,25 +7217,13 @@
       <c r="F26" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
-        <v>110</v>
-      </c>
-      <c r="M26" t="s">
-        <v>222</v>
-      </c>
-      <c r="N26" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="27" spans="1:14" ht="184" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="184" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>44</v>
@@ -7372,150 +7232,88 @@
         <v>8</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="F27" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H27"/>
-      <c r="I27" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J27" t="s">
-        <v>81</v>
-      </c>
-      <c r="K27" t="s">
-        <v>180</v>
-      </c>
-      <c r="L27" t="s">
-        <v>187</v>
-      </c>
-      <c r="M27" t="s">
-        <v>223</v>
-      </c>
-      <c r="N27" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="28" spans="1:14" ht="160" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F28" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G28" s="5"/>
       <c r="H28"/>
-      <c r="I28" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L28" t="s">
-        <v>110</v>
-      </c>
-      <c r="M28" t="s">
-        <v>224</v>
-      </c>
-      <c r="N28" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="29" spans="1:14" ht="208" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="F29" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H29"/>
-      <c r="I29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" t="s">
-        <v>81</v>
-      </c>
-      <c r="K29" t="s">
-        <v>181</v>
-      </c>
-      <c r="L29" t="s">
-        <v>114</v>
-      </c>
-      <c r="M29" t="s">
-        <v>225</v>
-      </c>
-      <c r="N29" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="30" spans="1:14" ht="304" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="304" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="F30" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G30" s="5"/>
       <c r="H30"/>
-      <c r="I30" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L30" t="s">
-        <v>193</v>
-      </c>
-      <c r="M30" t="s">
-        <v>226</v>
-      </c>
-      <c r="N30" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="31" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
@@ -7524,225 +7322,240 @@
         <v>8</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="F31" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G31" s="5"/>
       <c r="H31"/>
-      <c r="I31" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L31" t="s">
-        <v>193</v>
-      </c>
-      <c r="M31" t="s">
-        <v>227</v>
-      </c>
-      <c r="N31" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="32" spans="1:14" ht="166" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="166" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F32" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>160</v>
+      <c r="G32" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="H32"/>
-      <c r="I32" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" t="s">
-        <v>166</v>
-      </c>
-      <c r="K32" t="s">
-        <v>182</v>
-      </c>
-      <c r="L32" t="s">
-        <v>194</v>
-      </c>
-      <c r="M32" t="s">
-        <v>228</v>
-      </c>
-      <c r="N32" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="33" spans="1:14" ht="256" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="F33" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>162</v>
+      <c r="G33" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="H33"/>
-      <c r="I33" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33" t="s">
-        <v>87</v>
-      </c>
-      <c r="K33" t="s">
-        <v>183</v>
-      </c>
-      <c r="L33" t="s">
-        <v>195</v>
-      </c>
-      <c r="M33" t="s">
-        <v>229</v>
-      </c>
-      <c r="N33" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="34" spans="1:14" ht="256" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F34" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G34" s="5"/>
       <c r="H34"/>
-      <c r="I34" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L34" t="s">
-        <v>110</v>
-      </c>
-      <c r="M34" t="s">
-        <v>230</v>
-      </c>
-      <c r="N34" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="35" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F35" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G35" s="5"/>
       <c r="H35"/>
-      <c r="I35" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J35" t="s">
-        <v>81</v>
-      </c>
-      <c r="K35" t="s">
-        <v>184</v>
-      </c>
-      <c r="L35" t="s">
-        <v>192</v>
-      </c>
-      <c r="M35" t="s">
-        <v>231</v>
-      </c>
-      <c r="N35" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="36" spans="1:14" ht="288" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="F36" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H36"/>
-      <c r="I36" s="3" t="b">
+    </row>
+    <row r="37" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="11"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F38" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J36" t="s">
+      <c r="G38" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="K36" t="s">
-        <v>185</v>
-      </c>
-      <c r="L36" t="s">
-        <v>196</v>
-      </c>
-      <c r="M36" t="s">
-        <v>232</v>
-      </c>
-      <c r="N36" t="b">
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F39" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="G39" s="11"/>
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11"/>
+      <c r="H41"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>